<commit_message>
Delete Garett and New England from blanks
</commit_message>
<xml_diff>
--- a/blanks.xlsx
+++ b/blanks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dingjunwen/Downloads/Smith/heidivest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A61F157-27AE-CC46-B9B4-72C092A9DCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10190AD5-B044-CC4F-911D-628EA35B65CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12500" yWindow="1800" windowWidth="26540" windowHeight="11520" xr2:uid="{4F1F3C9B-DB5E-4EB6-AD1F-F2EB0579F72E}"/>
+    <workbookView xWindow="6000" yWindow="3500" windowWidth="26540" windowHeight="11520" xr2:uid="{4F1F3C9B-DB5E-4EB6-AD1F-F2EB0579F72E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t>UNITID</t>
   </si>
@@ -473,19 +473,13 @@
   </si>
   <si>
     <t>Emory University</t>
-  </si>
-  <si>
-    <t>Garrett-Evangelical Theological Seminary</t>
-  </si>
-  <si>
-    <t>University of New England</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,6 +507,18 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -534,10 +540,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -852,10 +860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B29692-5278-4CA4-879D-495E66DC3B21}">
-  <dimension ref="A1:B147"/>
+  <dimension ref="A1:B146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="A148" sqref="A148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1985,59 +1993,47 @@
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B141" s="1">
-        <v>145275</v>
+        <v>168342</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B142" s="1">
-        <v>168342</v>
+        <v>215062</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B143" s="1">
-        <v>161457</v>
+        <v>204501</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B144" s="1">
-        <v>215062</v>
+        <v>117946</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B145" s="1">
-        <v>204501</v>
+        <v>173258</v>
       </c>
     </row>
     <row r="146" spans="1:2">
-      <c r="A146" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B146" s="1">
-        <v>117946</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2">
-      <c r="A147" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B147" s="1">
-        <v>173258</v>
-      </c>
+      <c r="A146" s="3"/>
+      <c r="B146" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>